<commit_message>
adding variable to incorporate all environments
</commit_message>
<xml_diff>
--- a/Test Data/Smoke Pack Test Data.xlsx
+++ b/Test Data/Smoke Pack Test Data.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Cloud 01" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="26">
   <si>
     <t>Web Application URL</t>
   </si>
@@ -38,9 +38,6 @@
     <t>Branch User Password</t>
   </si>
   <si>
-    <t>password12</t>
-  </si>
-  <si>
     <t>Android Application path</t>
   </si>
   <si>
@@ -78,9 +75,6 @@
   </si>
   <si>
     <t>ChannelType</t>
-  </si>
-  <si>
-    <t>Large A Beauty</t>
   </si>
   <si>
     <t>Sales Return Sales Person</t>
@@ -375,8 +369,8 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -406,95 +400,95 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -512,7 +506,9 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -541,95 +537,95 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -647,7 +643,9 @@
   </sheetPr>
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
@@ -676,95 +674,95 @@
         <v>4</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>12</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>